<commit_message>
Instances up to S8
</commit_message>
<xml_diff>
--- a/instances/I1_S6_mean.xlsx
+++ b/instances/I1_S6_mean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\wm-stochastic\instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8A8BF6-23F4-4627-8B09-546DE10871B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8F6B6E-19FE-411E-BAA6-56346D51D3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="10104" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
     <t>s</t>
   </si>
   <si>
-    <t>I1_S5_mean</t>
+    <t>I1_S6_mean</t>
   </si>
 </sst>
 </file>
@@ -468,12 +468,12 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -481,7 +481,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -489,7 +489,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -497,7 +497,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -505,7 +505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -513,7 +513,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -521,7 +521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -529,7 +529,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -537,7 +537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -545,7 +545,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -553,7 +553,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -575,9 +575,9 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -588,7 +588,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -599,7 +599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -610,7 +610,7 @@
         <v>8.44</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -621,7 +621,7 @@
         <v>7.58</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -632,7 +632,7 @@
         <v>4.21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -643,7 +643,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -654,7 +654,7 @@
         <v>5.1100000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -665,7 +665,7 @@
         <v>4.05</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -676,7 +676,7 @@
         <v>7.84</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -687,7 +687,7 @@
         <v>3.03</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -698,7 +698,7 @@
         <v>4.7699999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -722,9 +722,9 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -738,7 +738,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -752,7 +752,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -766,7 +766,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -780,7 +780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -794,7 +794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -808,7 +808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -835,9 +835,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -848,7 +848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -859,7 +859,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -870,7 +870,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -894,9 +894,9 @@
       <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -904,7 +904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -912,7 +912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -920,7 +920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -928,7 +928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -936,7 +936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -944,7 +944,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -952,7 +952,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -960,7 +960,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -968,7 +968,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -976,7 +976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -997,9 +997,9 @@
       <selection activeCell="C2" sqref="C2:C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>16.591999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>7.4120000000000008</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>9.1959999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>9.5879999999999992</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>7.1099999999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>14.834</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>9.1720000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>6.1360000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>10.348000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>12.842000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>7.38</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>13.568</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>11.31</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>9.8780000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>6.36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>7.3739999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>13.295999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>10.646000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>13.292</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>8.0980000000000008</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>7</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>11.885999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>11.12</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>8</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>10.212</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>6.1319999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>9</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>8.4640000000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>9</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>11.16</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>7.1039999999999992</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>5.4979999999999993</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>10</v>
       </c>

</xml_diff>